<commit_message>
added column to soccer shoes wide
</commit_message>
<xml_diff>
--- a/data/soccer_shoes_wide.xlsx
+++ b/data/soccer_shoes_wide.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2220DB6-424D-45D6-AA5F-5E1A34735E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{723E3618-981A-49CF-BF01-EBF0EA8F4FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="1070" windowWidth="17250" windowHeight="8460" xr2:uid="{9D9638EA-10E3-3242-B778-8D8F864FEB58}"/>
+    <workbookView xWindow="-28920" yWindow="-8205" windowWidth="29040" windowHeight="16440" xr2:uid="{9D9638EA-10E3-3242-B778-8D8F864FEB58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>shoe_a</t>
   </si>
@@ -49,15 +49,46 @@
   </si>
   <si>
     <t>socks</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>These data are based on Figure 5 in the article:</t>
+  </si>
+  <si>
+    <t>The influence of soccer shoe design on playing performance: a series of</t>
+  </si>
+  <si>
+    <t>biomechanical studies</t>
+  </si>
+  <si>
+    <t>Ewald M. Hennig and Thorsten Sterzing</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Hennig, Ewald M. and Sterzing, Thorsten(2010) 'The influence of soccer shoe design on playing</t>
+  </si>
+  <si>
+    <t>performance: a series of biomechanical studies', Footwear Science, 2: 1, 3 — 11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -81,14 +112,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{313EB8F0-8C16-4728-9CF9-DBF707BD2C9B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -400,13 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A561CCF5-6956-6D42-BCFE-E6BDAE2C7AF7}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,8 +461,11 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>35</v>
       </c>
@@ -445,8 +484,11 @@
       <c r="F2">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>32</v>
       </c>
@@ -465,8 +507,11 @@
       <c r="F3">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>39</v>
       </c>
@@ -485,8 +530,11 @@
       <c r="F4">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>44</v>
       </c>
@@ -505,8 +553,11 @@
       <c r="F5">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>35</v>
       </c>
@@ -525,8 +576,11 @@
       <c r="F6">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>27</v>
       </c>
@@ -545,8 +599,11 @@
       <c r="F7">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>28</v>
       </c>
@@ -565,8 +622,11 @@
       <c r="F8">
         <v>41</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>31</v>
       </c>
@@ -586,7 +646,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>39</v>
       </c>
@@ -606,7 +666,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>38</v>
       </c>
@@ -626,7 +686,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>37</v>
       </c>
@@ -646,7 +706,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>34</v>
       </c>
@@ -666,7 +726,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>22</v>
       </c>
@@ -686,7 +746,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>29</v>
       </c>
@@ -706,7 +766,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>35</v>
       </c>

</xml_diff>